<commit_message>
practice programs added 03
</commit_message>
<xml_diff>
--- a/DS ALGO PRACTICE BUBBER/FINAL450 QUESTIONS OF DS ALGO.xlsx
+++ b/DS ALGO PRACTICE BUBBER/FINAL450 QUESTIONS OF DS ALGO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R\Desktop\new folder\DS ALGO PRACTICE BUBBER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86E8379-71E5-47BB-A895-75722428D00D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090279F6-C807-4C4A-A951-150D417D7A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1476" yWindow="1224" windowWidth="16800" windowHeight="9420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="0" yWindow="1596" windowWidth="16800" windowHeight="9420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1555,6 +1555,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1571,10 +1639,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="DEDEDE"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="181B28"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1866,7 +1934,7 @@
   <dimension ref="A1:C481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -1965,7 +2033,7 @@
         <v>11</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21">

</xml_diff>

<commit_message>
Adding more practiced files
</commit_message>
<xml_diff>
--- a/DS ALGO PRACTICE BUBBER/FINAL450 QUESTIONS OF DS ALGO.xlsx
+++ b/DS ALGO PRACTICE BUBBER/FINAL450 QUESTIONS OF DS ALGO.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\R\Desktop\new folder\DS ALGO PRACTICE BUBBER\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{090279F6-C807-4C4A-A951-150D417D7A22}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D299C525-ED96-4F0C-8818-E76D11EF1130}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1596" windowWidth="16800" windowHeight="9420" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
+    <workbookView xWindow="1212" yWindow="3240" windowWidth="16788" windowHeight="6432" xr2:uid="{261C335C-1D91-C143-AEEF-19B82073468C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1933,8 +1934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1CDA779-6CF2-8045-9DE0-880424A4EED5}">
   <dimension ref="A1:C481"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6"/>
@@ -2044,7 +2045,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21">
@@ -2055,7 +2056,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>4</v>
+        <v>465</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="21">

</xml_diff>